<commit_message>
Updated the BOM for the shoulder rot motor and its bearings and belt, the shoulder bearings
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nerd Projects\Exoskeleton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B29082-B87D-4A9B-98DB-4FE39994693A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E837A6D-CC96-4067-9EF9-F3E559BB64F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Name of Part</t>
   </si>
@@ -78,6 +78,27 @@
   </si>
   <si>
     <t>https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>Shouder Rotation Nema 23 50:1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0B5XQK5H1?ref=ppx_yo2ov_dt_b_fed_asin_title&amp;th=1</t>
+  </si>
+  <si>
+    <t>Shoulder Bearing - LM104949/11 * 2</t>
+  </si>
+  <si>
+    <t>Shoulder Rot Bearing - 368A/362A * 2</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07RW366QL?smid=A1THAZDOWP300U&amp;th=1</t>
+  </si>
+  <si>
+    <t>Shoulder Rot Belt - 6484K144</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/6484K144/</t>
   </si>
 </sst>
 </file>
@@ -460,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4691FD-8288-456A-8708-8A03D6C242A3}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,46 +530,94 @@
         <v>91.84</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>91.84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>31.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>37.78</v>
+      </c>
+    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>16.86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9">
+      <c r="D16">
         <v>42.14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10">
+      <c r="D17">
         <v>22.99</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11">
+      <c r="D18">
         <v>29.9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{7BA362F7-E062-4F13-951E-1165F7EFDA5F}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{B27905DD-BD52-4A50-9EFE-F0B0876AF13C}"/>
-    <hyperlink ref="C9" r:id="rId3" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
-    <hyperlink ref="C10" r:id="rId4" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
-    <hyperlink ref="C11" r:id="rId5" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
+    <hyperlink ref="C16" r:id="rId2" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
+    <hyperlink ref="C17" r:id="rId3" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
+    <hyperlink ref="C18" r:id="rId4" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{B27905DD-BD52-4A50-9EFE-F0B0876AF13C}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{1E01B732-0347-4C8D-90BC-75B6830128CC}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{E25FD138-1514-4141-AA28-4248FA5CC47D}"/>
+    <hyperlink ref="C7" r:id="rId8" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed the belt to a larger one
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nerd Projects\Exoskeleton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E837A6D-CC96-4067-9EF9-F3E559BB64F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5906A04-E293-4852-9AE4-017F1BD9AA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
   </bookViews>
@@ -95,10 +95,10 @@
     <t>https://www.amazon.com/gp/product/B07RW366QL?smid=A1THAZDOWP300U&amp;th=1</t>
   </si>
   <si>
-    <t>Shoulder Rot Belt - 6484K144</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/6484K144/</t>
+    <t>Shoulder Rot Belt - 6484K701</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/6484K701/</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +571,7 @@
         <v>20</v>
       </c>
       <c r="D9">
-        <v>16.86</v>
+        <v>18.62</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added elbow bearings into BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nerd Projects\Exoskeleton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5906A04-E293-4852-9AE4-017F1BD9AA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A013207-71A4-4572-AAD6-FE090A2AD8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Name of Part</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/6484K701/</t>
+  </si>
+  <si>
+    <t>Elbow Bearing - 2788/2720 * 2</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4691FD-8288-456A-8708-8A03D6C242A3}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -563,61 +569,73 @@
         <v>37.78</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>44.98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>18.62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16">
-        <v>42.14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D17">
-        <v>22.99</v>
+        <v>42.14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>22.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>29.9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{7BA362F7-E062-4F13-951E-1165F7EFDA5F}"/>
-    <hyperlink ref="C16" r:id="rId2" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
-    <hyperlink ref="C17" r:id="rId3" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
-    <hyperlink ref="C18" r:id="rId4" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
+    <hyperlink ref="C17" r:id="rId2" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
+    <hyperlink ref="C18" r:id="rId3" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
+    <hyperlink ref="C19" r:id="rId4" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
     <hyperlink ref="C3" r:id="rId5" xr:uid="{B27905DD-BD52-4A50-9EFE-F0B0876AF13C}"/>
     <hyperlink ref="C4" r:id="rId6" xr:uid="{1E01B732-0347-4C8D-90BC-75B6830128CC}"/>
     <hyperlink ref="C6" r:id="rId7" xr:uid="{E25FD138-1514-4141-AA28-4248FA5CC47D}"/>
     <hyperlink ref="C7" r:id="rId8" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
-    <hyperlink ref="C9" r:id="rId9" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
+    <hyperlink ref="C8" r:id="rId10" display="https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1" xr:uid="{FC47F6DC-E95B-4B1F-8B59-85F19DCB3094}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the BOM for screws and limit switches
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nerd Projects\Exoskeleton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A013207-71A4-4572-AAD6-FE090A2AD8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00EFA36-138D-45DE-978F-9857E3244461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Name of Part</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1</t>
+  </si>
+  <si>
+    <t>Bought?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Limit switches</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1</t>
+  </si>
+  <si>
+    <t>M5 x 100mm</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/iExcell-Metric-Stainless-Socket-Screws/dp/B09QKM2X5G?crid=2MK4MF236GEFN&amp;dib=eyJ2IjoiMSJ9.iC1dzNuElQeAGv8Q2ei-zZco6YxIBAktsmbyStzCqSFqd9r7lrorbtVyCUvNKisze0bdgeFbH96gusH1nNaL2A9Ws9ySpUU_ziywJx6X_ytnPE1xAHZNGk5Vl_HOGoVSMSG3g_B4V1yOe3wLc7JViaw-sQX8q1I4UVR3M5soo3Mxy2NqLfkZYgQW2q2Z-pIHong-4lpmMSEDJF8aiA_GIvubPNTl_qCemBnWyuJlODA.vA653d80XAMpYpFkrhwMNjq8kcmIksJEKgVBXtZhack&amp;dib_tag=se&amp;keywords=100mm%2BM5%2Bscrews&amp;qid=1750896856&amp;sprefix=10mm%2Bm5%2Bscrews%2Caps%2C190&amp;sr=8-1&amp;th=1</t>
   </si>
 </sst>
 </file>
@@ -487,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4691FD-8288-456A-8708-8A03D6C242A3}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +518,7 @@
     <col min="3" max="3" width="127.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,8 +531,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -525,7 +546,7 @@
         <v>91.84</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -536,7 +557,7 @@
         <v>91.84</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -547,7 +568,7 @@
         <v>91.84</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -557,8 +578,11 @@
       <c r="D6">
         <v>31.58</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -569,7 +593,7 @@
         <v>37.78</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -580,7 +604,7 @@
         <v>44.98</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -589,6 +613,31 @@
       </c>
       <c r="D10">
         <v>18.62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>9.56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <v>9.99</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -636,6 +685,8 @@
     <hyperlink ref="C7" r:id="rId8" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
     <hyperlink ref="C10" r:id="rId9" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
     <hyperlink ref="C8" r:id="rId10" display="https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1" xr:uid="{FC47F6DC-E95B-4B1F-8B59-85F19DCB3094}"/>
+    <hyperlink ref="C14" r:id="rId11" display="https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1" xr:uid="{B9D5167A-39E1-4B43-B027-77B3DA4F8773}"/>
+    <hyperlink ref="C12" r:id="rId12" display="https://www.amazon.com/iExcell-Metric-Stainless-Socket-Screws/dp/B09QKM2X5G?crid=2MK4MF236GEFN&amp;dib=eyJ2IjoiMSJ9.iC1dzNuElQeAGv8Q2ei-zZco6YxIBAktsmbyStzCqSFqd9r7lrorbtVyCUvNKisze0bdgeFbH96gusH1nNaL2A9Ws9ySpUU_ziywJx6X_ytnPE1xAHZNGk5Vl_HOGoVSMSG3g_B4V1yOe3wLc7JViaw-sQX8q1I4UVR3M5soo3Mxy2NqLfkZYgQW2q2Z-pIHong-4lpmMSEDJF8aiA_GIvubPNTl_qCemBnWyuJlODA.vA653d80XAMpYpFkrhwMNjq8kcmIksJEKgVBXtZhack&amp;dib_tag=se&amp;keywords=100mm%2BM5%2Bscrews&amp;qid=1750896856&amp;sprefix=10mm%2Bm5%2Bscrews%2Caps%2C190&amp;sr=8-1&amp;th=1" xr:uid="{FD36F02F-A655-41C1-8A83-17EC30B4C477}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the BOM by adding in bearings and new motors
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nerd Projects\Exoskeleton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00EFA36-138D-45DE-978F-9857E3244461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60313FCF-23D2-4B22-9F91-DC3918E4A97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Name of Part</t>
   </si>
@@ -47,21 +47,9 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Shoulder - Nema 23 100:1 Planetary Gearbox</t>
-  </si>
-  <si>
-    <t>Elbow - Nema 23 50:1 Planetary Gearbox</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
-    <t>https://www.omc-stepperonline.com/nema-23-stepper-motor-l-56mm-gear-ratio-50-1-high-precision-planetary-gearbox-23hs22-2804s-hg50</t>
-  </si>
-  <si>
-    <t>https://www.omc-stepperonline.com/nema-23-stepper-motor-l-56mm-gear-ratio-100-1-high-precision-planetary-gearbox-23hs22-2804s-hg100</t>
-  </si>
-  <si>
     <t>Position Tracker - BNO055</t>
   </si>
   <si>
@@ -80,9 +68,6 @@
     <t>https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1</t>
   </si>
   <si>
-    <t>Shouder Rotation Nema 23 50:1</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/dp/B0B5XQK5H1?ref=ppx_yo2ov_dt_b_fed_asin_title&amp;th=1</t>
   </si>
   <si>
@@ -123,6 +108,33 @@
   </si>
   <si>
     <t>https://www.amazon.com/iExcell-Metric-Stainless-Socket-Screws/dp/B09QKM2X5G?crid=2MK4MF236GEFN&amp;dib=eyJ2IjoiMSJ9.iC1dzNuElQeAGv8Q2ei-zZco6YxIBAktsmbyStzCqSFqd9r7lrorbtVyCUvNKisze0bdgeFbH96gusH1nNaL2A9Ws9ySpUU_ziywJx6X_ytnPE1xAHZNGk5Vl_HOGoVSMSG3g_B4V1yOe3wLc7JViaw-sQX8q1I4UVR3M5soo3Mxy2NqLfkZYgQW2q2Z-pIHong-4lpmMSEDJF8aiA_GIvubPNTl_qCemBnWyuJlODA.vA653d80XAMpYpFkrhwMNjq8kcmIksJEKgVBXtZhack&amp;dib_tag=se&amp;keywords=100mm%2BM5%2Bscrews&amp;qid=1750896856&amp;sprefix=10mm%2Bm5%2Bscrews%2Caps%2C190&amp;sr=8-1&amp;th=1</t>
+  </si>
+  <si>
+    <t>Shoulder - Nema 23 50:1 Planetary Gearbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shoulder Rotation - Nema 23 20:1 </t>
+  </si>
+  <si>
+    <t>https://www.omc-stepperonline.com/nema-23-closed-loop-stepper-motor-l-77mm-gear-ratio-20-1-high-precision-planetary-gearbox-23hs22-hg20-e1000</t>
+  </si>
+  <si>
+    <t>Forearm rot - Nema 17 20:1</t>
+  </si>
+  <si>
+    <t>https://www.omc-stepperonline.com/nema-17-closed-loop-stepper-motor-l-39mm-gear-ratio-20-1-high-precision-planetary-gearbox-17hs15-hg20-e1000</t>
+  </si>
+  <si>
+    <t>Elbow - Nema 23 20:1</t>
+  </si>
+  <si>
+    <t>https://www.omc-stepperonline.com/nema-23-closed-loop-stepper-motor-l-78mm-gear-ratio-50-1-high-precision-planetary-gearbox-23hs22-hg50-e1000</t>
+  </si>
+  <si>
+    <t>Forearm Bearing - 6812-2RS</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PSBTLP?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1</t>
   </si>
 </sst>
 </file>
@@ -505,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4691FD-8288-456A-8708-8A03D6C242A3}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,167 +538,191 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>91.84</v>
+        <v>74.14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D3">
-        <v>91.84</v>
+        <v>73.28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D4">
-        <v>91.84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>31.58</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
+        <v>73.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>55.75</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>37.78</v>
+        <v>31.58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D8">
+        <v>37.78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
         <v>44.98</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D10">
-        <v>18.62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
+        <v>14.09</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D12">
-        <v>9.56</v>
+        <v>18.62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D14">
+        <v>9.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16">
         <v>9.99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17">
-        <v>42.14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>22.99</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D19">
+        <v>42.14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>22.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21">
         <v>29.9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{7BA362F7-E062-4F13-951E-1165F7EFDA5F}"/>
-    <hyperlink ref="C17" r:id="rId2" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
-    <hyperlink ref="C18" r:id="rId3" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
-    <hyperlink ref="C19" r:id="rId4" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{B27905DD-BD52-4A50-9EFE-F0B0876AF13C}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{1E01B732-0347-4C8D-90BC-75B6830128CC}"/>
-    <hyperlink ref="C6" r:id="rId7" xr:uid="{E25FD138-1514-4141-AA28-4248FA5CC47D}"/>
-    <hyperlink ref="C7" r:id="rId8" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
-    <hyperlink ref="C8" r:id="rId10" display="https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1" xr:uid="{FC47F6DC-E95B-4B1F-8B59-85F19DCB3094}"/>
-    <hyperlink ref="C14" r:id="rId11" display="https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1" xr:uid="{B9D5167A-39E1-4B43-B027-77B3DA4F8773}"/>
-    <hyperlink ref="C12" r:id="rId12" display="https://www.amazon.com/iExcell-Metric-Stainless-Socket-Screws/dp/B09QKM2X5G?crid=2MK4MF236GEFN&amp;dib=eyJ2IjoiMSJ9.iC1dzNuElQeAGv8Q2ei-zZco6YxIBAktsmbyStzCqSFqd9r7lrorbtVyCUvNKisze0bdgeFbH96gusH1nNaL2A9Ws9ySpUU_ziywJx6X_ytnPE1xAHZNGk5Vl_HOGoVSMSG3g_B4V1yOe3wLc7JViaw-sQX8q1I4UVR3M5soo3Mxy2NqLfkZYgQW2q2Z-pIHong-4lpmMSEDJF8aiA_GIvubPNTl_qCemBnWyuJlODA.vA653d80XAMpYpFkrhwMNjq8kcmIksJEKgVBXtZhack&amp;dib_tag=se&amp;keywords=100mm%2BM5%2Bscrews&amp;qid=1750896856&amp;sprefix=10mm%2Bm5%2Bscrews%2Caps%2C190&amp;sr=8-1&amp;th=1" xr:uid="{FD36F02F-A655-41C1-8A83-17EC30B4C477}"/>
+    <hyperlink ref="C19" r:id="rId1" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
+    <hyperlink ref="C20" r:id="rId2" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
+    <hyperlink ref="C21" r:id="rId3" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{E25FD138-1514-4141-AA28-4248FA5CC47D}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
+    <hyperlink ref="C9" r:id="rId7" display="https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1" xr:uid="{FC47F6DC-E95B-4B1F-8B59-85F19DCB3094}"/>
+    <hyperlink ref="C16" r:id="rId8" display="https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1" xr:uid="{B9D5167A-39E1-4B43-B027-77B3DA4F8773}"/>
+    <hyperlink ref="C14" r:id="rId9" display="https://www.amazon.com/iExcell-Metric-Stainless-Socket-Screws/dp/B09QKM2X5G?crid=2MK4MF236GEFN&amp;dib=eyJ2IjoiMSJ9.iC1dzNuElQeAGv8Q2ei-zZco6YxIBAktsmbyStzCqSFqd9r7lrorbtVyCUvNKisze0bdgeFbH96gusH1nNaL2A9Ws9ySpUU_ziywJx6X_ytnPE1xAHZNGk5Vl_HOGoVSMSG3g_B4V1yOe3wLc7JViaw-sQX8q1I4UVR3M5soo3Mxy2NqLfkZYgQW2q2Z-pIHong-4lpmMSEDJF8aiA_GIvubPNTl_qCemBnWyuJlODA.vA653d80XAMpYpFkrhwMNjq8kcmIksJEKgVBXtZhack&amp;dib_tag=se&amp;keywords=100mm%2BM5%2Bscrews&amp;qid=1750896856&amp;sprefix=10mm%2Bm5%2Bscrews%2Caps%2C190&amp;sr=8-1&amp;th=1" xr:uid="{FD36F02F-A655-41C1-8A83-17EC30B4C477}"/>
+    <hyperlink ref="C3" r:id="rId10" xr:uid="{085862A1-697A-4933-A8B9-3EEE0F16855C}"/>
+    <hyperlink ref="C5" r:id="rId11" xr:uid="{310A8217-1D64-4225-95F2-44DFEACBAAAA}"/>
+    <hyperlink ref="C4" r:id="rId12" xr:uid="{73450F25-0AE8-405E-A571-D3E74B994BB1}"/>
+    <hyperlink ref="C2" r:id="rId13" xr:uid="{2B08A3BE-9C4A-40EA-8E3D-C61326F0789A}"/>
+    <hyperlink ref="C10" r:id="rId14" display="https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PSBTLP?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1" xr:uid="{00C7B0B6-295B-4A4C-9E8F-9CD459861A98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the BOM with wrist bearing and motor
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nerd Projects\Exoskeleton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60313FCF-23D2-4B22-9F91-DC3918E4A97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55213829-557F-4ECF-96B0-AD65BCA2A41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Name of Part</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PSBTLP?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1</t>
+  </si>
+  <si>
+    <t>Wrist Rot - Nema 17 20:1</t>
+  </si>
+  <si>
+    <t>Wrist Bearing -  6706-2RS</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PS9PHD?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1</t>
   </si>
 </sst>
 </file>
@@ -517,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4691FD-8288-456A-8708-8A03D6C242A3}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,138 +600,162 @@
         <v>55.75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>31.58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>55.75</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>37.78</v>
+        <v>31.58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>44.98</v>
+        <v>37.78</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>44.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>14.09</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D12">
-        <v>18.62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
+        <v>8.49</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D14">
-        <v>9.56</v>
+        <v>18.62</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>9.56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16">
+      <c r="D18">
         <v>9.99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>42.14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>22.99</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>42.14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>22.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>29.9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C19" r:id="rId1" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
-    <hyperlink ref="C20" r:id="rId2" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
-    <hyperlink ref="C21" r:id="rId3" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{E25FD138-1514-4141-AA28-4248FA5CC47D}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
-    <hyperlink ref="C12" r:id="rId6" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
-    <hyperlink ref="C9" r:id="rId7" display="https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1" xr:uid="{FC47F6DC-E95B-4B1F-8B59-85F19DCB3094}"/>
-    <hyperlink ref="C16" r:id="rId8" display="https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1" xr:uid="{B9D5167A-39E1-4B43-B027-77B3DA4F8773}"/>
-    <hyperlink ref="C14" r:id="rId9" display="https://www.amazon.com/iExcell-Metric-Stainless-Socket-Screws/dp/B09QKM2X5G?crid=2MK4MF236GEFN&amp;dib=eyJ2IjoiMSJ9.iC1dzNuElQeAGv8Q2ei-zZco6YxIBAktsmbyStzCqSFqd9r7lrorbtVyCUvNKisze0bdgeFbH96gusH1nNaL2A9Ws9ySpUU_ziywJx6X_ytnPE1xAHZNGk5Vl_HOGoVSMSG3g_B4V1yOe3wLc7JViaw-sQX8q1I4UVR3M5soo3Mxy2NqLfkZYgQW2q2Z-pIHong-4lpmMSEDJF8aiA_GIvubPNTl_qCemBnWyuJlODA.vA653d80XAMpYpFkrhwMNjq8kcmIksJEKgVBXtZhack&amp;dib_tag=se&amp;keywords=100mm%2BM5%2Bscrews&amp;qid=1750896856&amp;sprefix=10mm%2Bm5%2Bscrews%2Caps%2C190&amp;sr=8-1&amp;th=1" xr:uid="{FD36F02F-A655-41C1-8A83-17EC30B4C477}"/>
+    <hyperlink ref="C21" r:id="rId1" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
+    <hyperlink ref="C22" r:id="rId2" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
+    <hyperlink ref="C23" r:id="rId3" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{E25FD138-1514-4141-AA28-4248FA5CC47D}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
+    <hyperlink ref="C14" r:id="rId6" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
+    <hyperlink ref="C10" r:id="rId7" display="https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1" xr:uid="{FC47F6DC-E95B-4B1F-8B59-85F19DCB3094}"/>
+    <hyperlink ref="C18" r:id="rId8" display="https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1" xr:uid="{B9D5167A-39E1-4B43-B027-77B3DA4F8773}"/>
+    <hyperlink ref="C16" r:id="rId9" display="https://www.amazon.com/iExcell-Metric-Stainless-Socket-Screws/dp/B09QKM2X5G?crid=2MK4MF236GEFN&amp;dib=eyJ2IjoiMSJ9.iC1dzNuElQeAGv8Q2ei-zZco6YxIBAktsmbyStzCqSFqd9r7lrorbtVyCUvNKisze0bdgeFbH96gusH1nNaL2A9Ws9ySpUU_ziywJx6X_ytnPE1xAHZNGk5Vl_HOGoVSMSG3g_B4V1yOe3wLc7JViaw-sQX8q1I4UVR3M5soo3Mxy2NqLfkZYgQW2q2Z-pIHong-4lpmMSEDJF8aiA_GIvubPNTl_qCemBnWyuJlODA.vA653d80XAMpYpFkrhwMNjq8kcmIksJEKgVBXtZhack&amp;dib_tag=se&amp;keywords=100mm%2BM5%2Bscrews&amp;qid=1750896856&amp;sprefix=10mm%2Bm5%2Bscrews%2Caps%2C190&amp;sr=8-1&amp;th=1" xr:uid="{FD36F02F-A655-41C1-8A83-17EC30B4C477}"/>
     <hyperlink ref="C3" r:id="rId10" xr:uid="{085862A1-697A-4933-A8B9-3EEE0F16855C}"/>
     <hyperlink ref="C5" r:id="rId11" xr:uid="{310A8217-1D64-4225-95F2-44DFEACBAAAA}"/>
     <hyperlink ref="C4" r:id="rId12" xr:uid="{73450F25-0AE8-405E-A571-D3E74B994BB1}"/>
     <hyperlink ref="C2" r:id="rId13" xr:uid="{2B08A3BE-9C4A-40EA-8E3D-C61326F0789A}"/>
-    <hyperlink ref="C10" r:id="rId14" display="https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PSBTLP?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1" xr:uid="{00C7B0B6-295B-4A4C-9E8F-9CD459861A98}"/>
+    <hyperlink ref="C11" r:id="rId14" display="https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PSBTLP?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1" xr:uid="{00C7B0B6-295B-4A4C-9E8F-9CD459861A98}"/>
+    <hyperlink ref="C6" r:id="rId15" xr:uid="{C2CA6759-75F6-4512-B657-03EDD135DE7F}"/>
+    <hyperlink ref="C12" r:id="rId16" display="https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PS9PHD?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1" xr:uid="{C4761357-6142-45EB-91FD-DBD1CD8BA7B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Switched out the wrong bearing link for the shoulder rot
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nerd Projects\Exoskeleton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55213829-557F-4ECF-96B0-AD65BCA2A41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A4A346-997B-4111-8AF9-ADE5F1D464D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
   </bookViews>
@@ -74,12 +74,6 @@
     <t>Shoulder Bearing - LM104949/11 * 2</t>
   </si>
   <si>
-    <t>Shoulder Rot Bearing - 368A/362A * 2</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B07RW366QL?smid=A1THAZDOWP300U&amp;th=1</t>
-  </si>
-  <si>
     <t>Shoulder Rot Belt - 6484K701</t>
   </si>
   <si>
@@ -144,6 +138,12 @@
   </si>
   <si>
     <t>https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PS9PHD?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Timken-SET37-Tapered-Roller-Bearing/dp/B000BZ6YEK?crid=2UVMW157QN9VD&amp;dib=eyJ2IjoiMSJ9.2iRD0--LwAOtK6sCHU59ccwGJuRc5xFBYyjJQh18M4UXnO7H_ZEp_RF1DBAneDyUPEW41QxDKmbDABDOTskGcetuw5M7rczrcJk2ijXBzWPzPx4e81ycuzjMNTUf1LCgl8F85OwKQvS0FSy3HqugdxaoWSM9lra-DHRZzyeZ4RZV037QmoTEjlaHqrlmwPh9t85RVao1pSw0P0kDZEYdu48P_FysqfBYEduzfz9srAsN7hSKuiP0O7mAwPilwJhbmhWH6cM_JCfLtP8VQdRd-V7lYpPKFxGmKKUMIfvId7g.83HkNvFnLf5ILJIPVbD65pyGfEMhvFL6FLQp0veUnws&amp;dib_tag=se&amp;keywords=tapered+roller+bearing&amp;qid=1751500342&amp;s=industrial&amp;sprefix=tapered+roller+beairn%2Cindustrial%2C164&amp;sr=1-6</t>
+  </si>
+  <si>
+    <t>Shoulder Rot Bearing - SET37 * 2</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,15 +553,15 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>74.14</v>
@@ -569,10 +569,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>73.28</v>
@@ -580,10 +580,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>73.28</v>
@@ -591,10 +591,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <v>55.75</v>
@@ -602,10 +602,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>55.75</v>
@@ -622,26 +622,26 @@
         <v>31.58</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D9">
-        <v>37.78</v>
+        <v>35.36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>44.98</v>
@@ -649,10 +649,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>14.09</v>
@@ -660,10 +660,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>8.49</v>
@@ -671,24 +671,24 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <v>18.62</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D16">
         <v>9.56</v>
@@ -696,10 +696,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18">
         <v>9.99</v>
@@ -744,7 +744,7 @@
     <hyperlink ref="C22" r:id="rId2" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
     <hyperlink ref="C23" r:id="rId3" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
     <hyperlink ref="C8" r:id="rId4" xr:uid="{E25FD138-1514-4141-AA28-4248FA5CC47D}"/>
-    <hyperlink ref="C9" r:id="rId5" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
+    <hyperlink ref="C9" r:id="rId5" display="https://www.amazon.com/Timken-SET37-Tapered-Roller-Bearing/dp/B000BZ6YEK?crid=2UVMW157QN9VD&amp;dib=eyJ2IjoiMSJ9.2iRD0--LwAOtK6sCHU59ccwGJuRc5xFBYyjJQh18M4UXnO7H_ZEp_RF1DBAneDyUPEW41QxDKmbDABDOTskGcetuw5M7rczrcJk2ijXBzWPzPx4e81ycuzjMNTUf1LCgl8F85OwKQvS0FSy3HqugdxaoWSM9lra-DHRZzyeZ4RZV037QmoTEjlaHqrlmwPh9t85RVao1pSw0P0kDZEYdu48P_FysqfBYEduzfz9srAsN7hSKuiP0O7mAwPilwJhbmhWH6cM_JCfLtP8VQdRd-V7lYpPKFxGmKKUMIfvId7g.83HkNvFnLf5ILJIPVbD65pyGfEMhvFL6FLQp0veUnws&amp;dib_tag=se&amp;keywords=tapered+roller+bearing&amp;qid=1751500342&amp;s=industrial&amp;sprefix=tapered+roller+beairn%2Cindustrial%2C164&amp;sr=1-6" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
     <hyperlink ref="C14" r:id="rId6" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
     <hyperlink ref="C10" r:id="rId7" display="https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1" xr:uid="{FC47F6DC-E95B-4B1F-8B59-85F19DCB3094}"/>
     <hyperlink ref="C18" r:id="rId8" display="https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1" xr:uid="{B9D5167A-39E1-4B43-B027-77B3DA4F8773}"/>

</xml_diff>

<commit_message>
Fixed the price typo for the shoulder elbow bearing
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nerd Projects\Exoskeleton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A4A346-997B-4111-8AF9-ADE5F1D464D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812F2A1B-C0C0-4AC9-9258-6FFA826572FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
+    <workbookView minimized="1" xWindow="6510" yWindow="3390" windowWidth="21600" windowHeight="11385" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4691FD-8288-456A-8708-8A03D6C242A3}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +644,7 @@
         <v>15</v>
       </c>
       <c r="D10">
-        <v>44.98</v>
+        <v>22.49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Replaced the arduino with the Teensy and updated the buy status of some components
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nerd Projects\Exoskeleton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812F2A1B-C0C0-4AC9-9258-6FFA826572FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939E5946-5103-4CD4-806F-4F9A5F873C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6510" yWindow="3390" windowWidth="21600" windowHeight="11385" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93390776-EE1A-4C57-BB21-0FF6FB39352F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Name of Part</t>
   </si>
@@ -56,18 +56,6 @@
     <t>https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor</t>
   </si>
   <si>
-    <t>MCU - Arduino Mega</t>
-  </si>
-  <si>
-    <t>Breakout Board For Arduino Mega</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/dp/B0B5XQK5H1?ref=ppx_yo2ov_dt_b_fed_asin_title&amp;th=1</t>
   </si>
   <si>
@@ -98,12 +86,6 @@
     <t>https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1</t>
   </si>
   <si>
-    <t>M5 x 100mm</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/iExcell-Metric-Stainless-Socket-Screws/dp/B09QKM2X5G?crid=2MK4MF236GEFN&amp;dib=eyJ2IjoiMSJ9.iC1dzNuElQeAGv8Q2ei-zZco6YxIBAktsmbyStzCqSFqd9r7lrorbtVyCUvNKisze0bdgeFbH96gusH1nNaL2A9Ws9ySpUU_ziywJx6X_ytnPE1xAHZNGk5Vl_HOGoVSMSG3g_B4V1yOe3wLc7JViaw-sQX8q1I4UVR3M5soo3Mxy2NqLfkZYgQW2q2Z-pIHong-4lpmMSEDJF8aiA_GIvubPNTl_qCemBnWyuJlODA.vA653d80XAMpYpFkrhwMNjq8kcmIksJEKgVBXtZhack&amp;dib_tag=se&amp;keywords=100mm%2BM5%2Bscrews&amp;qid=1750896856&amp;sprefix=10mm%2Bm5%2Bscrews%2Caps%2C190&amp;sr=8-1&amp;th=1</t>
-  </si>
-  <si>
     <t>Shoulder - Nema 23 50:1 Planetary Gearbox</t>
   </si>
   <si>
@@ -144,6 +126,18 @@
   </si>
   <si>
     <t>Shoulder Rot Bearing - SET37 * 2</t>
+  </si>
+  <si>
+    <t>Teensy 4.1</t>
+  </si>
+  <si>
+    <t>Teensy 4.1 Breakout Board</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/PJRC-Teensy-4-1-with-Pins/dp/B08CTM3279?crid=34THGHK8HI5A5&amp;dib=eyJ2IjoiMSJ9.SbX6rnuR22BHW7UQV6IYcVquOHgAcfF6FDHlv7GM_vKT9MZOutc6v8JDNGdhQhbiYP4uJ-ih0NO1rzKtU8ke5Gc6_bJxzp7ev6EG7waNf17z4a0L7rdyFvU7ThnQ4rgkUBqPCNRUZoPtGvpYWM19fn2RM2zND9cgGb-SO14ajYjJNK9JYGkhWhwTlOHYc60nYDfhsQpsOz0Gv2QFw1gXQzylB_ye0_Q0QifIXi9xSttaUNt1dcZz_9g9VRpqZIMgdQ38K8K7nNSNBsh2-ZbcAroQTeOViLv20zAN8XElNRA.dH0FLKLGjCNqvZAP7ix9dN2o4ETagPELIxq-ZSTjPGQ&amp;dib_tag=se&amp;keywords=teensy+4.1&amp;qid=1752095247&amp;s=electronics&amp;sprefix=teensy+4.%2Celectronics%2C166&amp;sr=1-2</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Terminal-Breakout-Module-Teensy-Version/dp/B08R7P8G9X?crid=RFAES7QZ4Q4L&amp;dib=eyJ2IjoiMSJ9.EmBJYSUPM1Px4iZIZ4bLaeXFC9dBP04lmedi1rosx1b99wYfBTwe_VV8NOpVGGOv0VKc0cRl9KQSf7qFGasCC59KAZVHhDLAZpdVwNjYpp-wYIBK9A-IxRjA9Y9-15-ZHQMlmtqLGbhui1ytjpQMCcrBUHHNwiGs0YiuMmUotlpZ-HIF79JLI9_QlCbyPlze81DvjdiJPpToWqvGgnPUzwU6oWsxs9ujaMuysafF3GI.s-LjX6BPIAq2uzQRqiWLnRgsl93d0zz9KPEnz1vPS-U&amp;dib_tag=se&amp;keywords=teensy+4.1+breakout+board&amp;qid=1752095278&amp;sprefix=teensy+4.1+breakout+board%2Caps%2C170&amp;sr=8-3</t>
   </si>
 </sst>
 </file>
@@ -526,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4691FD-8288-456A-8708-8A03D6C242A3}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,26 +547,29 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D2">
         <v>74.14</v>
       </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>73.28</v>
@@ -580,10 +577,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>73.28</v>
@@ -591,10 +588,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>55.75</v>
@@ -602,10 +599,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>55.75</v>
@@ -613,149 +610,156 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>31.58</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <v>35.36</v>
       </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>22.49</v>
       </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>14.09</v>
       </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <v>8.49</v>
       </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <v>18.62</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16">
-        <v>9.56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
         <v>9.99</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>42.14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D21">
-        <v>42.14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44.15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D22">
-        <v>22.99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23">
-        <v>29.9</v>
+        <v>23.9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C21" r:id="rId1" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
-    <hyperlink ref="C22" r:id="rId2" display="https://www.amazon.com/ELEGOO-Compatible-Arduino-Projects-Compliant/dp/B01H4ZLZLQ?crid=1J7XJ0X0LQPVN&amp;dib=eyJ2IjoiMSJ9.C9li7QlUOdnawgCr8xZlUWZQDyHFpesFSB7DviVllKqGmMMk5K-VvRQhyhHA4AqyscubrPU9wtPQy7VaCUKyuO3EYxuwrXTtMddGGzmxhz2PsRzMuvE8bAxqUv28A2LO06Tke-rB36vSu9bQf09V1GC7pj5uKZzQJkLdic9dUJnzrOmyLS-h0Mapf2ito6gkx7mB0lzZBfwz7Se5A46tey_XF6O_qB5_P7jwQ0n3ykA.LeEpybFPF8KLznW1_yr7GJ-aAyT_db2aS0qKXnS1gmQ&amp;dib_tag=se&amp;keywords=arduino+mega&amp;qid=1748287251&amp;sprefix=arduino+m%2Caps%2C196&amp;sr=8-1" xr:uid="{AEB30628-B873-4EC5-85F5-0E2F3EC84500}"/>
-    <hyperlink ref="C23" r:id="rId3" display="https://www.amazon.com/Electronics-Salon-Terminal-Breakout-Arduino-MEGA-2560/dp/B07H9TJCWN?crid=3GOXBFMIMGAN5&amp;dib=eyJ2IjoiMSJ9.3XoGINQ1IkjC7gxdNc2ljQUBQiGFRTxo6wcllu5zLJD4S5M_-a9LJcrYRsXXQWHM48vWvwebUTPYqNItuzPCHNEWmF_yUpMQKUkhu-itZOA2c2Cxf59eIFpwTYJ2f0jn0uPzD1N9kueUxKdz7t-9UC3upY-8wkvC1O3fa9MiE_LeQYs69F45wXyXzklh5Vy_W5L5hLnv2jeDA8_EWCDZzhZn5VQvzMYVrzc09GHfXxQ.CMbmQ7q0axvhf8XS3yt9uEAiVMgr_RdX5OyNJsZCLc0&amp;dib_tag=se&amp;keywords=arduino+mega+breakout+board&amp;qid=1748287276&amp;sprefix=arduino+mega+b%2Caps%2C174&amp;sr=8-1" xr:uid="{9444E3DA-8FAD-4110-9519-5E3E93BD7C12}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{E25FD138-1514-4141-AA28-4248FA5CC47D}"/>
-    <hyperlink ref="C9" r:id="rId5" display="https://www.amazon.com/Timken-SET37-Tapered-Roller-Bearing/dp/B000BZ6YEK?crid=2UVMW157QN9VD&amp;dib=eyJ2IjoiMSJ9.2iRD0--LwAOtK6sCHU59ccwGJuRc5xFBYyjJQh18M4UXnO7H_ZEp_RF1DBAneDyUPEW41QxDKmbDABDOTskGcetuw5M7rczrcJk2ijXBzWPzPx4e81ycuzjMNTUf1LCgl8F85OwKQvS0FSy3HqugdxaoWSM9lra-DHRZzyeZ4RZV037QmoTEjlaHqrlmwPh9t85RVao1pSw0P0kDZEYdu48P_FysqfBYEduzfz9srAsN7hSKuiP0O7mAwPilwJhbmhWH6cM_JCfLtP8VQdRd-V7lYpPKFxGmKKUMIfvId7g.83HkNvFnLf5ILJIPVbD65pyGfEMhvFL6FLQp0veUnws&amp;dib_tag=se&amp;keywords=tapered+roller+bearing&amp;qid=1751500342&amp;s=industrial&amp;sprefix=tapered+roller+beairn%2Cindustrial%2C164&amp;sr=1-6" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
-    <hyperlink ref="C14" r:id="rId6" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
-    <hyperlink ref="C10" r:id="rId7" display="https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1" xr:uid="{FC47F6DC-E95B-4B1F-8B59-85F19DCB3094}"/>
-    <hyperlink ref="C18" r:id="rId8" display="https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1" xr:uid="{B9D5167A-39E1-4B43-B027-77B3DA4F8773}"/>
-    <hyperlink ref="C16" r:id="rId9" display="https://www.amazon.com/iExcell-Metric-Stainless-Socket-Screws/dp/B09QKM2X5G?crid=2MK4MF236GEFN&amp;dib=eyJ2IjoiMSJ9.iC1dzNuElQeAGv8Q2ei-zZco6YxIBAktsmbyStzCqSFqd9r7lrorbtVyCUvNKisze0bdgeFbH96gusH1nNaL2A9Ws9ySpUU_ziywJx6X_ytnPE1xAHZNGk5Vl_HOGoVSMSG3g_B4V1yOe3wLc7JViaw-sQX8q1I4UVR3M5soo3Mxy2NqLfkZYgQW2q2Z-pIHong-4lpmMSEDJF8aiA_GIvubPNTl_qCemBnWyuJlODA.vA653d80XAMpYpFkrhwMNjq8kcmIksJEKgVBXtZhack&amp;dib_tag=se&amp;keywords=100mm%2BM5%2Bscrews&amp;qid=1750896856&amp;sprefix=10mm%2Bm5%2Bscrews%2Caps%2C190&amp;sr=8-1&amp;th=1" xr:uid="{FD36F02F-A655-41C1-8A83-17EC30B4C477}"/>
-    <hyperlink ref="C3" r:id="rId10" xr:uid="{085862A1-697A-4933-A8B9-3EEE0F16855C}"/>
-    <hyperlink ref="C5" r:id="rId11" xr:uid="{310A8217-1D64-4225-95F2-44DFEACBAAAA}"/>
-    <hyperlink ref="C4" r:id="rId12" xr:uid="{73450F25-0AE8-405E-A571-D3E74B994BB1}"/>
-    <hyperlink ref="C2" r:id="rId13" xr:uid="{2B08A3BE-9C4A-40EA-8E3D-C61326F0789A}"/>
-    <hyperlink ref="C11" r:id="rId14" display="https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PSBTLP?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1" xr:uid="{00C7B0B6-295B-4A4C-9E8F-9CD459861A98}"/>
-    <hyperlink ref="C6" r:id="rId15" xr:uid="{C2CA6759-75F6-4512-B657-03EDD135DE7F}"/>
-    <hyperlink ref="C12" r:id="rId16" display="https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PS9PHD?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1" xr:uid="{C4761357-6142-45EB-91FD-DBD1CD8BA7B6}"/>
+    <hyperlink ref="C20" r:id="rId1" location="averageCustomerReviewsAnchor" display="https://www.amazon.com/Adafruit-Absolute-Orientation-Fusion-Breakout/dp/B017PEIGIG?crid=3J1S4PG236LH9&amp;dib=eyJ2IjoiMSJ9.b_9piN2jpFgVdQUKUlO--RmT6WlwK-qAMknMAnS5IS0iWy-_pnTiR3lz6vGtzAZ-QU1RgFWmLARA63BbYm2iJgMJAs6M1k6BiQz6U9YyVjStz_rtSVCSfxwNcbItqNjUWQ-LD3Trq2PqxcLGdjeZ6dK9118d_v6FfAvXVBp5GxVkAJRjcc1m__B_8t4cydOF6rnBGZeh3U4aBQFniM8blFVuth9Mlcic1U3wytci0Ls.w2QFliZTY50PWL6_lk2pkuIYw4gKKLWDaw-qPCEKXlg&amp;dib_tag=se&amp;keywords=BNO055&amp;qid=1748287133&amp;sprefix=bno05%2Caps%2C183&amp;sr=8-3#averageCustomerReviewsAnchor" xr:uid="{2B05B596-7F99-41C0-BBA5-EDFDD8C96EFD}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{E25FD138-1514-4141-AA28-4248FA5CC47D}"/>
+    <hyperlink ref="C9" r:id="rId3" display="https://www.amazon.com/Timken-SET37-Tapered-Roller-Bearing/dp/B000BZ6YEK?crid=2UVMW157QN9VD&amp;dib=eyJ2IjoiMSJ9.2iRD0--LwAOtK6sCHU59ccwGJuRc5xFBYyjJQh18M4UXnO7H_ZEp_RF1DBAneDyUPEW41QxDKmbDABDOTskGcetuw5M7rczrcJk2ijXBzWPzPx4e81ycuzjMNTUf1LCgl8F85OwKQvS0FSy3HqugdxaoWSM9lra-DHRZzyeZ4RZV037QmoTEjlaHqrlmwPh9t85RVao1pSw0P0kDZEYdu48P_FysqfBYEduzfz9srAsN7hSKuiP0O7mAwPilwJhbmhWH6cM_JCfLtP8VQdRd-V7lYpPKFxGmKKUMIfvId7g.83HkNvFnLf5ILJIPVbD65pyGfEMhvFL6FLQp0veUnws&amp;dib_tag=se&amp;keywords=tapered+roller+bearing&amp;qid=1751500342&amp;s=industrial&amp;sprefix=tapered+roller+beairn%2Cindustrial%2C164&amp;sr=1-6" xr:uid="{53C683BF-D541-4716-BD0B-11043D03AB57}"/>
+    <hyperlink ref="C14" r:id="rId4" xr:uid="{382AB26D-2F13-448A-9A25-0F46E8448152}"/>
+    <hyperlink ref="C10" r:id="rId5" display="https://www.amazon.com/uxcell-Tapered-Roller-Bearing-Width/dp/B0B5XQX2RD?crid=XEE741AKFTOD&amp;dib=eyJ2IjoiMSJ9.DswnWR3W53Ca9cwH4GaxUPFfJg6uabw9uJwooYlFrzk7jzzlfG_MR0SsAizypRTTbxfEGlJpdYcGXDXn75oN1tfidCPGbHF7eAhr06xiHk1JEg9I9tQ5WpIR7Ey0jD_-TdYD1oo7D927GMhQ9Tolso8enodh4dCep77Z58otH--bhgN7hrswT6TSPZT1pWZTq4AFg6dcLr53SGj7WlGqL7Rqs3bs78WDBd7gsg1-6vM.f28EI9GGTBJBW6Tif3erxd-Ub8gBTqe45Gfaa4eA8E4&amp;dib_tag=se&amp;keywords=roller%2Btapered%2Bbearing&amp;qid=1750119672&amp;sprefix=roller%2Btapered%2Bbeari%2Caps%2C169&amp;sr=8-9&amp;th=1" xr:uid="{FC47F6DC-E95B-4B1F-8B59-85F19DCB3094}"/>
+    <hyperlink ref="C17" r:id="rId6" display="https://www.amazon.com/JANDECCN-Switch-Straight-Action-V-153-1C25/dp/B09SWCJ8FF?crid=2MA83SE8988B5&amp;dib=eyJ2IjoiMSJ9.FPAndwd916JYq_epoDDZGiqAa4E79JO0OJPmLzVPG4LVDe_BYuWJ1g0hMND_l7lLAk2blrJqCF_h8BzsxraJsgmFhKlRTBzc9Tmfbl1BoBjfOmF-oZg7L99hziyExQJ-hQ6ONFWY85dl22ioUJ6LoeD-plLm227aK9kfQAPHV1h7h4SwjvRjRxq-JqFEBz39LxdExxOrFczEOY1lPgUymlz_8USo84ze_x_tXcTnwao.WhA46og7gWEunQjyywSUpuTHSFrAkRIclqMocdDKJbk&amp;dib_tag=se&amp;keywords=limit%2Bswitch&amp;qid=1750810216&amp;sprefix=limit%2Bswitc%2Caps%2C164&amp;sr=8-5&amp;th=1" xr:uid="{B9D5167A-39E1-4B43-B027-77B3DA4F8773}"/>
+    <hyperlink ref="C3" r:id="rId7" xr:uid="{085862A1-697A-4933-A8B9-3EEE0F16855C}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{310A8217-1D64-4225-95F2-44DFEACBAAAA}"/>
+    <hyperlink ref="C4" r:id="rId9" xr:uid="{73450F25-0AE8-405E-A571-D3E74B994BB1}"/>
+    <hyperlink ref="C2" r:id="rId10" xr:uid="{2B08A3BE-9C4A-40EA-8E3D-C61326F0789A}"/>
+    <hyperlink ref="C11" r:id="rId11" display="https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PSBTLP?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1" xr:uid="{00C7B0B6-295B-4A4C-9E8F-9CD459861A98}"/>
+    <hyperlink ref="C6" r:id="rId12" xr:uid="{C2CA6759-75F6-4512-B657-03EDD135DE7F}"/>
+    <hyperlink ref="C12" r:id="rId13" display="https://www.amazon.com/uxcell-6806-2RS-Groove-Bearings-Double/dp/B082PS9PHD?crid=343XO74UUMOR8&amp;dib=eyJ2IjoiMSJ9.usjalkOILuax4NzDfSCcKZKlIcvuBJ6141WDs0F_w7JM4ltP-r8--wyHD9ffJsM-qEB_nj0XxxmOpIGXu54oOr3wPLi9JyWqqzNuamxdJTJPyUrGWaztFiwG0FUqrTXkCe0-wx78My4sc22vxg62M2Tj0pjbmoGSb6cgtYRmstLOZoICuXRgpazt9XjmvsoHPfYr7-D3EXRBTaBrErEr9W_xgNp1ft09nWRyKoIvXcE.hJIMcmy-iUTeCoKT1D0KrQQjv09h0jiJkZxQlAhD7DA&amp;dib_tag=se&amp;keywords=bal%2Bbearing%2B30mm&amp;qid=1750968982&amp;sprefix=bal%2Bbearing%2B30mm%2Caps%2C206&amp;sr=8-3&amp;th=1" xr:uid="{C4761357-6142-45EB-91FD-DBD1CD8BA7B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>